<commit_message>
👷 2nd bunch of cleaning updates - renaming functions - updating gui defaults
</commit_message>
<xml_diff>
--- a/01_EFForTS-ABM/EFForTS-ABM_parameters_and_output.xlsx
+++ b/01_EFForTS-ABM/EFForTS-ABM_parameters_and_output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\owncloud\git\EFForTS-ABM\01_EFForTS-ABM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\owncloud\git_efforts\EFForTS-ABM\01_EFForTS-ABM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BD81EE-C3E9-4EEC-9681-2F5B20484B5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87426F28-4B30-4A3E-8AFB-F7D00388C2D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21870" yWindow="360" windowWidth="23820" windowHeight="19425" xr2:uid="{CCAD1C1C-E277-4675-834D-1499CE7B176B}"/>
+    <workbookView xWindow="27150" yWindow="1425" windowWidth="18165" windowHeight="18060" xr2:uid="{CCAD1C1C-E277-4675-834D-1499CE7B176B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="178">
   <si>
     <t>group</t>
   </si>
@@ -116,9 +116,6 @@
     <t>price_scenario</t>
   </si>
   <si>
-    <t>"historical_trends"</t>
-  </si>
-  <si>
     <t>price-fluctuation-percent</t>
   </si>
   <si>
@@ -290,12 +287,6 @@
     <t>hhage</t>
   </si>
   <si>
-    <t>calc_bird_richness?</t>
-  </si>
-  <si>
-    <t>invest_plantdiv?</t>
-  </si>
-  <si>
     <t>biodiversity</t>
   </si>
   <si>
@@ -552,6 +543,30 @@
   </si>
   <si>
     <t>h_connected_hhs</t>
+  </si>
+  <si>
+    <t>"constant_prices"</t>
+  </si>
+  <si>
+    <t>biodiv_birds</t>
+  </si>
+  <si>
+    <t>"none"</t>
+  </si>
+  <si>
+    <t>biodiv_plants</t>
+  </si>
+  <si>
+    <t>"SAR"</t>
+  </si>
+  <si>
+    <t>biodiv_invest_objective</t>
+  </si>
+  <si>
+    <t>"generell"</t>
+  </si>
+  <si>
+    <t>ecol_biodiv_interval</t>
   </si>
 </sst>
 </file>
@@ -912,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9AA953-A8CF-47CE-B234-B31FEC912566}">
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,12 +1080,12 @@
         <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -1090,7 +1105,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -1110,7 +1125,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -1125,12 +1140,12 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -1150,7 +1165,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -1170,7 +1185,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -1190,7 +1205,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -1205,12 +1220,12 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -1230,7 +1245,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -1250,7 +1265,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -1270,16 +1285,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>41</v>
       </c>
       <c r="E18" t="s">
         <v>17</v>
@@ -1290,7 +1305,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
@@ -1299,7 +1314,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -1310,7 +1325,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -1319,7 +1334,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
@@ -1330,7 +1345,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -1339,7 +1354,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1350,7 +1365,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -1359,7 +1374,7 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
         <v>17</v>
@@ -1370,7 +1385,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
@@ -1379,18 +1394,18 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s">
         <v>17</v>
       </c>
       <c r="F23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
@@ -1399,18 +1414,18 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
@@ -1419,7 +1434,7 @@
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
         <v>11</v>
@@ -1430,7 +1445,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -1439,7 +1454,7 @@
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1450,16 +1465,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
         <v>50</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>51</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
@@ -1470,7 +1485,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -1479,7 +1494,7 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1490,7 +1505,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
@@ -1499,7 +1514,7 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E29" t="s">
         <v>17</v>
@@ -1510,7 +1525,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
@@ -1519,18 +1534,18 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E30" t="s">
         <v>11</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
@@ -1539,7 +1554,7 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
@@ -1550,7 +1565,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
@@ -1559,7 +1574,7 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E32" t="s">
         <v>11</v>
@@ -1570,7 +1585,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
         <v>1</v>
@@ -1579,27 +1594,27 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E33" t="s">
         <v>20</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
         <v>59</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>60</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
@@ -1610,7 +1625,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -1619,18 +1634,18 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E35" t="s">
         <v>20</v>
       </c>
       <c r="F35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
@@ -1639,7 +1654,7 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
@@ -1650,7 +1665,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
@@ -1659,7 +1674,7 @@
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E37" t="s">
         <v>11</v>
@@ -1670,7 +1685,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
@@ -1679,7 +1694,7 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E38" t="s">
         <v>11</v>
@@ -1690,7 +1705,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
@@ -1699,7 +1714,7 @@
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E39" t="s">
         <v>11</v>
@@ -1710,16 +1725,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
         <v>67</v>
-      </c>
-      <c r="B40" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
-        <v>68</v>
       </c>
       <c r="E40" t="s">
         <v>11</v>
@@ -1730,7 +1745,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
@@ -1739,7 +1754,7 @@
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E41" t="s">
         <v>11</v>
@@ -1750,7 +1765,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
@@ -1759,7 +1774,7 @@
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E42" t="s">
         <v>11</v>
@@ -1770,7 +1785,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
@@ -1779,7 +1794,7 @@
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E43" t="s">
         <v>11</v>
@@ -1790,7 +1805,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
@@ -1799,7 +1814,7 @@
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E44" t="s">
         <v>11</v>
@@ -1810,7 +1825,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
         <v>1</v>
@@ -1819,7 +1834,7 @@
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E45" t="s">
         <v>11</v>
@@ -1830,7 +1845,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -1839,7 +1854,7 @@
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E46" t="s">
         <v>11</v>
@@ -1850,16 +1865,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
         <v>76</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>77</v>
       </c>
       <c r="E47" t="s">
         <v>11</v>
@@ -1870,7 +1885,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
@@ -1879,7 +1894,7 @@
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E48" t="s">
         <v>11</v>
@@ -1890,7 +1905,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
@@ -1899,7 +1914,7 @@
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E49" t="s">
         <v>11</v>
@@ -1910,7 +1925,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
@@ -1919,7 +1934,7 @@
         <v>4</v>
       </c>
       <c r="D50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E50" t="s">
         <v>11</v>
@@ -1930,7 +1945,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
@@ -1939,7 +1954,7 @@
         <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E51" t="s">
         <v>11</v>
@@ -1950,7 +1965,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B52" t="s">
         <v>1</v>
@@ -1959,7 +1974,7 @@
         <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E52" t="s">
         <v>11</v>
@@ -1970,16 +1985,16 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
         <v>83</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" t="s">
-        <v>84</v>
       </c>
       <c r="E53" t="s">
         <v>11</v>
@@ -1990,7 +2005,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>177</v>
       </c>
       <c r="B54" t="s">
         <v>1</v>
@@ -1999,18 +2014,18 @@
         <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E54" t="s">
-        <v>17</v>
-      </c>
-      <c r="F54" t="b">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="B55" t="s">
         <v>1</v>
@@ -2019,18 +2034,18 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E55" t="s">
-        <v>17</v>
-      </c>
-      <c r="F55" t="b">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="F55" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
       <c r="B56" t="s">
         <v>1</v>
@@ -2039,18 +2054,18 @@
         <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E56" t="s">
-        <v>17</v>
-      </c>
-      <c r="F56" t="b">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="F56" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>90</v>
+        <v>175</v>
       </c>
       <c r="B57" t="s">
         <v>1</v>
@@ -2059,18 +2074,18 @@
         <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E57" t="s">
-        <v>17</v>
-      </c>
-      <c r="F57" t="b">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="F57" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B58" t="s">
         <v>1</v>
@@ -2079,7 +2094,7 @@
         <v>4</v>
       </c>
       <c r="D58" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="E58" t="s">
         <v>17</v>
@@ -2090,7 +2105,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B59" t="s">
         <v>1</v>
@@ -2099,7 +2114,7 @@
         <v>4</v>
       </c>
       <c r="D59" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E59" t="s">
         <v>17</v>
@@ -2110,7 +2125,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
         <v>1</v>
@@ -2119,7 +2134,7 @@
         <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E60" t="s">
         <v>17</v>
@@ -2130,16 +2145,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
         <v>94</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" t="s">
-        <v>97</v>
       </c>
       <c r="E61" t="s">
         <v>17</v>
@@ -2150,7 +2165,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
@@ -2159,18 +2174,18 @@
         <v>4</v>
       </c>
       <c r="D62" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E62" t="s">
         <v>17</v>
       </c>
       <c r="F62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
         <v>1</v>
@@ -2179,58 +2194,58 @@
         <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E63" t="s">
         <v>17</v>
       </c>
       <c r="F63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B64" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C64" t="s">
         <v>4</v>
       </c>
       <c r="D64" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="F64" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B65" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
         <v>4</v>
       </c>
       <c r="D65" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E65" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="F65" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B66" t="s">
         <v>2</v>
@@ -2239,7 +2254,7 @@
         <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="E66" t="s">
         <v>11</v>
@@ -2250,7 +2265,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B67" t="s">
         <v>2</v>
@@ -2259,7 +2274,7 @@
         <v>4</v>
       </c>
       <c r="D67" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="E67" t="s">
         <v>11</v>
@@ -2270,7 +2285,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B68" t="s">
         <v>2</v>
@@ -2279,7 +2294,7 @@
         <v>4</v>
       </c>
       <c r="D68" t="s">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="E68" t="s">
         <v>11</v>
@@ -2290,7 +2305,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B69" t="s">
         <v>2</v>
@@ -2299,7 +2314,7 @@
         <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="E69" t="s">
         <v>11</v>
@@ -2310,7 +2325,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B70" t="s">
         <v>2</v>
@@ -2319,7 +2334,7 @@
         <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="E70" t="s">
         <v>11</v>
@@ -2330,7 +2345,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B71" t="s">
         <v>2</v>
@@ -2339,7 +2354,7 @@
         <v>4</v>
       </c>
       <c r="D71" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="E71" t="s">
         <v>11</v>
@@ -2350,7 +2365,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B72" t="s">
         <v>2</v>
@@ -2370,7 +2385,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B73" t="s">
         <v>2</v>
@@ -2390,7 +2405,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B74" t="s">
         <v>2</v>
@@ -2399,7 +2414,7 @@
         <v>4</v>
       </c>
       <c r="D74" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="E74" t="s">
         <v>11</v>
@@ -2410,7 +2425,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B75" t="s">
         <v>2</v>
@@ -2419,7 +2434,7 @@
         <v>4</v>
       </c>
       <c r="D75" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="E75" t="s">
         <v>11</v>
@@ -2430,7 +2445,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B76" t="s">
         <v>2</v>
@@ -2439,7 +2454,7 @@
         <v>4</v>
       </c>
       <c r="D76" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E76" t="s">
         <v>11</v>
@@ -2450,7 +2465,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B77" t="s">
         <v>2</v>
@@ -2459,7 +2474,7 @@
         <v>4</v>
       </c>
       <c r="D77" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E77" t="s">
         <v>11</v>
@@ -2470,7 +2485,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B78" t="s">
         <v>2</v>
@@ -2479,7 +2494,7 @@
         <v>4</v>
       </c>
       <c r="D78" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E78" t="s">
         <v>11</v>
@@ -2490,7 +2505,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B79" t="s">
         <v>2</v>
@@ -2499,7 +2514,7 @@
         <v>4</v>
       </c>
       <c r="D79" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E79" t="s">
         <v>11</v>
@@ -2510,7 +2525,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B80" t="s">
         <v>2</v>
@@ -2519,7 +2534,7 @@
         <v>4</v>
       </c>
       <c r="D80" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="E80" t="s">
         <v>11</v>
@@ -2530,7 +2545,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B81" t="s">
         <v>2</v>
@@ -2539,7 +2554,7 @@
         <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="E81" t="s">
         <v>11</v>
@@ -2550,7 +2565,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B82" t="s">
         <v>2</v>
@@ -2559,7 +2574,7 @@
         <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="E82" t="s">
         <v>11</v>
@@ -2570,7 +2585,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B83" t="s">
         <v>2</v>
@@ -2590,7 +2605,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B84" t="s">
         <v>2</v>
@@ -2610,16 +2625,16 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B85" t="s">
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D85" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="E85" t="s">
         <v>11</v>
@@ -2630,16 +2645,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B86" t="s">
         <v>2</v>
       </c>
       <c r="C86" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D86" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="E86" t="s">
         <v>11</v>
@@ -2650,7 +2665,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B87" t="s">
         <v>2</v>
@@ -2659,7 +2674,7 @@
         <v>5</v>
       </c>
       <c r="D87" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E87" t="s">
         <v>11</v>
@@ -2670,7 +2685,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B88" t="s">
         <v>2</v>
@@ -2679,7 +2694,7 @@
         <v>5</v>
       </c>
       <c r="D88" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E88" t="s">
         <v>11</v>
@@ -2690,7 +2705,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B89" t="s">
         <v>2</v>
@@ -2699,7 +2714,7 @@
         <v>5</v>
       </c>
       <c r="D89" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="E89" t="s">
         <v>11</v>
@@ -2710,7 +2725,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B90" t="s">
         <v>2</v>
@@ -2719,7 +2734,7 @@
         <v>5</v>
       </c>
       <c r="D90" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E90" t="s">
         <v>11</v>
@@ -2730,7 +2745,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B91" t="s">
         <v>2</v>
@@ -2739,7 +2754,7 @@
         <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="E91" t="s">
         <v>11</v>
@@ -2750,7 +2765,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B92" t="s">
         <v>2</v>
@@ -2759,7 +2774,7 @@
         <v>5</v>
       </c>
       <c r="D92" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E92" t="s">
         <v>11</v>
@@ -2770,7 +2785,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B93" t="s">
         <v>2</v>
@@ -2779,7 +2794,7 @@
         <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="E93" t="s">
         <v>11</v>
@@ -2790,7 +2805,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B94" t="s">
         <v>2</v>
@@ -2799,10 +2814,10 @@
         <v>5</v>
       </c>
       <c r="D94" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E94" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="F94" t="s">
         <v>12</v>
@@ -2810,7 +2825,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B95" t="s">
         <v>2</v>
@@ -2819,7 +2834,7 @@
         <v>5</v>
       </c>
       <c r="D95" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E95" t="s">
         <v>11</v>
@@ -2830,7 +2845,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B96" t="s">
         <v>2</v>
@@ -2839,10 +2854,10 @@
         <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="E96" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="F96" t="s">
         <v>12</v>
@@ -2850,7 +2865,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B97" t="s">
         <v>2</v>
@@ -2859,7 +2874,7 @@
         <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E97" t="s">
         <v>11</v>
@@ -2870,7 +2885,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B98" t="s">
         <v>2</v>
@@ -2890,7 +2905,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B99" t="s">
         <v>2</v>
@@ -2899,7 +2914,7 @@
         <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="E99" t="s">
         <v>11</v>
@@ -2910,7 +2925,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B100" t="s">
         <v>2</v>
@@ -2930,7 +2945,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B101" t="s">
         <v>2</v>
@@ -2950,7 +2965,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B102" t="s">
         <v>2</v>
@@ -2970,7 +2985,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B103" t="s">
         <v>2</v>
@@ -2990,16 +3005,16 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B104" t="s">
         <v>2</v>
       </c>
       <c r="C104" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D104" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="E104" t="s">
         <v>11</v>
@@ -3010,19 +3025,19 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B105" t="s">
         <v>2</v>
       </c>
       <c r="C105" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D105" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="E105" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="F105" t="s">
         <v>12</v>
@@ -3030,7 +3045,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B106" t="s">
         <v>2</v>
@@ -3039,7 +3054,7 @@
         <v>6</v>
       </c>
       <c r="D106" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E106" t="s">
         <v>11</v>
@@ -3050,7 +3065,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B107" t="s">
         <v>2</v>
@@ -3059,10 +3074,10 @@
         <v>6</v>
       </c>
       <c r="D107" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="E107" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="F107" t="s">
         <v>12</v>
@@ -3070,7 +3085,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B108" t="s">
         <v>2</v>
@@ -3079,7 +3094,7 @@
         <v>6</v>
       </c>
       <c r="D108" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E108" t="s">
         <v>11</v>
@@ -3090,7 +3105,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B109" t="s">
         <v>2</v>
@@ -3099,10 +3114,10 @@
         <v>6</v>
       </c>
       <c r="D109" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E109" t="s">
-        <v>165</v>
+        <v>11</v>
       </c>
       <c r="F109" t="s">
         <v>12</v>
@@ -3110,7 +3125,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B110" t="s">
         <v>2</v>
@@ -3119,10 +3134,10 @@
         <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E110" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F110" t="s">
         <v>12</v>
@@ -3130,7 +3145,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B111" t="s">
         <v>2</v>
@@ -3139,10 +3154,10 @@
         <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="E111" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
       <c r="F111" t="s">
         <v>12</v>
@@ -3150,7 +3165,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B112" t="s">
         <v>2</v>
@@ -3159,10 +3174,10 @@
         <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="E112" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F112" t="s">
         <v>12</v>
@@ -3170,7 +3185,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="B113" t="s">
         <v>2</v>
@@ -3179,7 +3194,7 @@
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E113" t="s">
         <v>11</v>
@@ -3190,7 +3205,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B114" t="s">
         <v>2</v>
@@ -3199,7 +3214,7 @@
         <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E114" t="s">
         <v>11</v>
@@ -3210,7 +3225,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="B115" t="s">
         <v>2</v>
@@ -3219,7 +3234,7 @@
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E115" t="s">
         <v>11</v>
@@ -3230,7 +3245,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B116" t="s">
         <v>2</v>
@@ -3239,7 +3254,7 @@
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="E116" t="s">
         <v>11</v>
@@ -3250,7 +3265,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B117" t="s">
         <v>2</v>
@@ -3259,7 +3274,7 @@
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="E117" t="s">
         <v>11</v>
@@ -3270,7 +3285,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B118" t="s">
         <v>2</v>
@@ -3279,7 +3294,7 @@
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="E118" t="s">
         <v>11</v>
@@ -3290,7 +3305,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B119" t="s">
         <v>2</v>
@@ -3299,7 +3314,7 @@
         <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="E119" t="s">
         <v>11</v>
@@ -3310,7 +3325,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B120" t="s">
         <v>2</v>
@@ -3319,7 +3334,7 @@
         <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E120" t="s">
         <v>11</v>
@@ -3330,7 +3345,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B121" t="s">
         <v>2</v>
@@ -3339,7 +3354,7 @@
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>158</v>
+        <v>40</v>
       </c>
       <c r="E121" t="s">
         <v>11</v>
@@ -3350,7 +3365,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B122" t="s">
         <v>2</v>
@@ -3359,7 +3374,7 @@
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>158</v>
+        <v>40</v>
       </c>
       <c r="E122" t="s">
         <v>11</v>
@@ -3370,7 +3385,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B123" t="s">
         <v>2</v>
@@ -3379,7 +3394,7 @@
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E123" t="s">
         <v>11</v>
@@ -3390,7 +3405,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B124" t="s">
         <v>2</v>
@@ -3399,7 +3414,7 @@
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E124" t="s">
         <v>11</v>
@@ -3410,7 +3425,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B125" t="s">
         <v>2</v>
@@ -3419,7 +3434,7 @@
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E125" t="s">
         <v>11</v>
@@ -3430,7 +3445,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B126" t="s">
         <v>2</v>
@@ -3439,7 +3454,7 @@
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="E126" t="s">
         <v>11</v>
@@ -3450,7 +3465,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B127" t="s">
         <v>2</v>
@@ -3459,7 +3474,7 @@
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="E127" t="s">
         <v>11</v>
@@ -3470,7 +3485,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B128" t="s">
         <v>2</v>
@@ -3479,10 +3494,10 @@
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="E128" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F128" t="s">
         <v>12</v>
@@ -3490,7 +3505,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B129" t="s">
         <v>2</v>
@@ -3499,7 +3514,7 @@
         <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="E129" t="s">
         <v>11</v>
@@ -3510,7 +3525,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B130" t="s">
         <v>2</v>
@@ -3519,7 +3534,7 @@
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="E130" t="s">
         <v>10</v>
@@ -3530,7 +3545,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B131" t="s">
         <v>2</v>
@@ -3539,10 +3554,10 @@
         <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="E131" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F131" t="s">
         <v>12</v>
@@ -3550,7 +3565,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B132" t="s">
         <v>2</v>
@@ -3559,12 +3574,52 @@
         <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="E132" t="s">
-        <v>165</v>
+        <v>10</v>
       </c>
       <c r="F132" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>166</v>
+      </c>
+      <c r="B133" t="s">
+        <v>2</v>
+      </c>
+      <c r="C133" t="s">
+        <v>6</v>
+      </c>
+      <c r="D133" t="s">
+        <v>14</v>
+      </c>
+      <c r="E133" t="s">
+        <v>10</v>
+      </c>
+      <c r="F133" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>169</v>
+      </c>
+      <c r="B134" t="s">
+        <v>2</v>
+      </c>
+      <c r="C134" t="s">
+        <v>6</v>
+      </c>
+      <c r="D134" t="s">
+        <v>50</v>
+      </c>
+      <c r="E134" t="s">
+        <v>162</v>
+      </c>
+      <c r="F134" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🎨 added new implemented parameters and varibales into parameters-excel file
</commit_message>
<xml_diff>
--- a/01_EFForTS-ABM/EFForTS-ABM_parameters_and_output.xlsx
+++ b/01_EFForTS-ABM/EFForTS-ABM_parameters_and_output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\owncloud\git_efforts\EFForTS-ABM\01_EFForTS-ABM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuliaHenzler\Documents\5_GitHub\EFForTS-ABM\01_EFForTS-ABM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87426F28-4B30-4A3E-8AFB-F7D00388C2D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1068FF-AFB2-41B5-9FD9-0F372F0456E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27150" yWindow="1425" windowWidth="18165" windowHeight="18060" xr2:uid="{CCAD1C1C-E277-4675-834D-1499CE7B176B}"/>
+    <workbookView xWindow="27150" yWindow="1430" windowWidth="18170" windowHeight="18060" xr2:uid="{CCAD1C1C-E277-4675-834D-1499CE7B176B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="185">
   <si>
     <t>group</t>
   </si>
@@ -567,6 +559,27 @@
   </si>
   <si>
     <t>ecol_biodiv_interval</t>
+  </si>
+  <si>
+    <t>p_landuse_invest</t>
+  </si>
+  <si>
+    <t>p_impact-location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patches </t>
+  </si>
+  <si>
+    <t>p_habitat_quality</t>
+  </si>
+  <si>
+    <t>landscape-hq</t>
+  </si>
+  <si>
+    <t>impact_all</t>
+  </si>
+  <si>
+    <t>dist_max</t>
   </si>
 </sst>
 </file>
@@ -927,23 +940,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9AA953-A8CF-47CE-B234-B31FEC912566}">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -963,7 +976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -983,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1003,7 +1016,7 @@
         <v>3478436</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1023,7 +1036,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1043,7 +1056,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1063,7 +1076,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1083,7 +1096,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1103,7 +1116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1123,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1143,7 +1156,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1163,7 +1176,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1183,7 +1196,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1203,7 +1216,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1223,7 +1236,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1243,7 +1256,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1263,7 +1276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1283,7 +1296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1303,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1323,7 +1336,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1343,7 +1356,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1363,7 +1376,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1383,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1403,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1423,7 +1436,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1443,7 +1456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1463,7 +1476,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1483,7 +1496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1503,7 +1516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1523,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -1543,7 +1556,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -1563,7 +1576,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -1583,7 +1596,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -1603,7 +1616,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -1623,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>61</v>
       </c>
@@ -1643,7 +1656,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>62</v>
       </c>
@@ -1663,7 +1676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -1683,7 +1696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>64</v>
       </c>
@@ -1703,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -1723,7 +1736,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -1743,7 +1756,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -1763,7 +1776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -1783,7 +1796,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -1803,7 +1816,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -1823,7 +1836,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>73</v>
       </c>
@@ -1843,7 +1856,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>74</v>
       </c>
@@ -1863,7 +1876,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>75</v>
       </c>
@@ -1883,7 +1896,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -1903,7 +1916,7 @@
         <v>14.24</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -1923,7 +1936,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -1943,7 +1956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -1963,7 +1976,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>81</v>
       </c>
@@ -1983,7 +1996,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>82</v>
       </c>
@@ -2003,7 +2016,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>177</v>
       </c>
@@ -2023,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>171</v>
       </c>
@@ -2043,7 +2056,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>173</v>
       </c>
@@ -2063,7 +2076,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>175</v>
       </c>
@@ -2083,38 +2096,38 @@
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>183</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>84</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>85</v>
       </c>
-      <c r="B58" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
         <v>86</v>
-      </c>
-      <c r="E58" t="s">
-        <v>17</v>
-      </c>
-      <c r="F58" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>87</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" t="s">
-        <v>94</v>
       </c>
       <c r="E59" t="s">
         <v>17</v>
@@ -2123,9 +2136,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
         <v>1</v>
@@ -2143,9 +2156,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
         <v>1</v>
@@ -2163,9 +2176,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
@@ -2183,9 +2196,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B63" t="s">
         <v>1</v>
@@ -2203,9 +2216,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B64" t="s">
         <v>1</v>
@@ -2220,12 +2233,12 @@
         <v>17</v>
       </c>
       <c r="F64" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B65" t="s">
         <v>1</v>
@@ -2243,29 +2256,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>94</v>
+      </c>
+      <c r="E66" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>95</v>
-      </c>
-      <c r="B66" t="s">
-        <v>2</v>
-      </c>
-      <c r="C66" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" t="s">
-        <v>96</v>
-      </c>
-      <c r="E66" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>97</v>
       </c>
       <c r="B67" t="s">
         <v>2</v>
@@ -2283,29 +2296,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>97</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>96</v>
+      </c>
+      <c r="E68" t="s">
+        <v>11</v>
+      </c>
+      <c r="F68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>98</v>
-      </c>
-      <c r="B68" t="s">
-        <v>2</v>
-      </c>
-      <c r="C68" t="s">
-        <v>4</v>
-      </c>
-      <c r="D68" t="s">
-        <v>13</v>
-      </c>
-      <c r="E68" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>99</v>
       </c>
       <c r="B69" t="s">
         <v>2</v>
@@ -2323,29 +2336,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>99</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>100</v>
-      </c>
-      <c r="B70" t="s">
-        <v>2</v>
-      </c>
-      <c r="C70" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" t="s">
-        <v>101</v>
-      </c>
-      <c r="E70" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>102</v>
       </c>
       <c r="B71" t="s">
         <v>2</v>
@@ -2363,29 +2376,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>102</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>101</v>
+      </c>
+      <c r="E72" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>103</v>
-      </c>
-      <c r="B72" t="s">
-        <v>2</v>
-      </c>
-      <c r="C72" t="s">
-        <v>4</v>
-      </c>
-      <c r="D72" t="s">
-        <v>14</v>
-      </c>
-      <c r="E72" t="s">
-        <v>11</v>
-      </c>
-      <c r="F72" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>104</v>
       </c>
       <c r="B73" t="s">
         <v>2</v>
@@ -2403,9 +2416,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B74" t="s">
         <v>2</v>
@@ -2423,9 +2436,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B75" t="s">
         <v>2</v>
@@ -2443,29 +2456,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
+        <v>106</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>14</v>
+      </c>
+      <c r="E76" t="s">
+        <v>11</v>
+      </c>
+      <c r="F76" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>107</v>
-      </c>
-      <c r="B76" t="s">
-        <v>2</v>
-      </c>
-      <c r="C76" t="s">
-        <v>4</v>
-      </c>
-      <c r="D76" t="s">
-        <v>108</v>
-      </c>
-      <c r="E76" t="s">
-        <v>11</v>
-      </c>
-      <c r="F76" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>109</v>
       </c>
       <c r="B77" t="s">
         <v>2</v>
@@ -2483,9 +2496,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B78" t="s">
         <v>2</v>
@@ -2503,9 +2516,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B79" t="s">
         <v>2</v>
@@ -2523,9 +2536,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B80" t="s">
         <v>2</v>
@@ -2543,9 +2556,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B81" t="s">
         <v>2</v>
@@ -2563,49 +2576,49 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" t="s">
+        <v>108</v>
+      </c>
+      <c r="E82" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>114</v>
       </c>
-      <c r="B82" t="s">
-        <v>2</v>
-      </c>
-      <c r="C82" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" t="s">
         <v>84</v>
       </c>
-      <c r="E82" t="s">
-        <v>11</v>
-      </c>
-      <c r="F82" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="E83" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>115</v>
-      </c>
-      <c r="B83" t="s">
-        <v>2</v>
-      </c>
-      <c r="C83" t="s">
-        <v>4</v>
-      </c>
-      <c r="D83" t="s">
-        <v>14</v>
-      </c>
-      <c r="E83" t="s">
-        <v>11</v>
-      </c>
-      <c r="F83" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>116</v>
       </c>
       <c r="B84" t="s">
         <v>2</v>
@@ -2623,9 +2636,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B85" t="s">
         <v>2</v>
@@ -2643,9 +2656,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B86" t="s">
         <v>2</v>
@@ -2663,69 +2676,69 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
+        <v>118</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" t="s">
+        <v>14</v>
+      </c>
+      <c r="E87" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>182</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2</v>
+      </c>
+      <c r="C88" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" t="s">
+        <v>84</v>
+      </c>
+      <c r="E88" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>184</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" t="s">
+        <v>84</v>
+      </c>
+      <c r="E89" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>119</v>
-      </c>
-      <c r="B87" t="s">
-        <v>2</v>
-      </c>
-      <c r="C87" t="s">
-        <v>5</v>
-      </c>
-      <c r="D87" t="s">
-        <v>101</v>
-      </c>
-      <c r="E87" t="s">
-        <v>11</v>
-      </c>
-      <c r="F87" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>120</v>
-      </c>
-      <c r="B88" t="s">
-        <v>2</v>
-      </c>
-      <c r="C88" t="s">
-        <v>5</v>
-      </c>
-      <c r="D88" t="s">
-        <v>101</v>
-      </c>
-      <c r="E88" t="s">
-        <v>11</v>
-      </c>
-      <c r="F88" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>121</v>
-      </c>
-      <c r="B89" t="s">
-        <v>2</v>
-      </c>
-      <c r="C89" t="s">
-        <v>5</v>
-      </c>
-      <c r="D89" t="s">
-        <v>101</v>
-      </c>
-      <c r="E89" t="s">
-        <v>11</v>
-      </c>
-      <c r="F89" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>122</v>
       </c>
       <c r="B90" t="s">
         <v>2</v>
@@ -2743,9 +2756,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B91" t="s">
         <v>2</v>
@@ -2754,7 +2767,7 @@
         <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="E91" t="s">
         <v>11</v>
@@ -2763,9 +2776,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B92" t="s">
         <v>2</v>
@@ -2783,9 +2796,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B93" t="s">
         <v>2</v>
@@ -2794,7 +2807,7 @@
         <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="E93" t="s">
         <v>11</v>
@@ -2803,9 +2816,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B94" t="s">
         <v>2</v>
@@ -2814,7 +2827,7 @@
         <v>5</v>
       </c>
       <c r="D94" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E94" t="s">
         <v>11</v>
@@ -2823,9 +2836,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B95" t="s">
         <v>2</v>
@@ -2834,7 +2847,7 @@
         <v>5</v>
       </c>
       <c r="D95" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E95" t="s">
         <v>11</v>
@@ -2843,9 +2856,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B96" t="s">
         <v>2</v>
@@ -2854,18 +2867,18 @@
         <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="E96" t="s">
-        <v>161</v>
+        <v>11</v>
       </c>
       <c r="F96" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B97" t="s">
         <v>2</v>
@@ -2874,7 +2887,7 @@
         <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E97" t="s">
         <v>11</v>
@@ -2883,9 +2896,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B98" t="s">
         <v>2</v>
@@ -2894,7 +2907,7 @@
         <v>5</v>
       </c>
       <c r="D98" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="E98" t="s">
         <v>11</v>
@@ -2903,9 +2916,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B99" t="s">
         <v>2</v>
@@ -2914,18 +2927,18 @@
         <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E99" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="F99" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B100" t="s">
         <v>2</v>
@@ -2934,7 +2947,7 @@
         <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="E100" t="s">
         <v>11</v>
@@ -2943,9 +2956,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B101" t="s">
         <v>2</v>
@@ -2963,9 +2976,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B102" t="s">
         <v>2</v>
@@ -2974,7 +2987,7 @@
         <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="E102" t="s">
         <v>11</v>
@@ -2983,9 +2996,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B103" t="s">
         <v>2</v>
@@ -3003,9 +3016,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B104" t="s">
         <v>2</v>
@@ -3023,9 +3036,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B105" t="s">
         <v>2</v>
@@ -3043,129 +3056,129 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>135</v>
+      </c>
+      <c r="B106" t="s">
+        <v>2</v>
+      </c>
+      <c r="C106" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" t="s">
+        <v>14</v>
+      </c>
+      <c r="E106" t="s">
+        <v>11</v>
+      </c>
+      <c r="F106" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>136</v>
+      </c>
+      <c r="B107" t="s">
+        <v>2</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" t="s">
+        <v>14</v>
+      </c>
+      <c r="E107" t="s">
+        <v>11</v>
+      </c>
+      <c r="F107" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>137</v>
+      </c>
+      <c r="B108" t="s">
+        <v>2</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" t="s">
+        <v>14</v>
+      </c>
+      <c r="E108" t="s">
+        <v>11</v>
+      </c>
+      <c r="F108" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>178</v>
+      </c>
+      <c r="B109" t="s">
+        <v>2</v>
+      </c>
+      <c r="C109" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109" t="s">
+        <v>84</v>
+      </c>
+      <c r="E109" t="s">
+        <v>11</v>
+      </c>
+      <c r="F109" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>179</v>
+      </c>
+      <c r="B110" t="s">
+        <v>2</v>
+      </c>
+      <c r="C110" t="s">
+        <v>180</v>
+      </c>
+      <c r="D110" t="s">
+        <v>84</v>
+      </c>
+      <c r="E110" t="s">
+        <v>17</v>
+      </c>
+      <c r="F110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>181</v>
+      </c>
+      <c r="B111" t="s">
+        <v>2</v>
+      </c>
+      <c r="C111" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" t="s">
+        <v>84</v>
+      </c>
+      <c r="E111" t="s">
+        <v>11</v>
+      </c>
+      <c r="F111" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>138</v>
-      </c>
-      <c r="B106" t="s">
-        <v>2</v>
-      </c>
-      <c r="C106" t="s">
-        <v>6</v>
-      </c>
-      <c r="D106" t="s">
-        <v>108</v>
-      </c>
-      <c r="E106" t="s">
-        <v>11</v>
-      </c>
-      <c r="F106" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>139</v>
-      </c>
-      <c r="B107" t="s">
-        <v>2</v>
-      </c>
-      <c r="C107" t="s">
-        <v>6</v>
-      </c>
-      <c r="D107" t="s">
-        <v>108</v>
-      </c>
-      <c r="E107" t="s">
-        <v>161</v>
-      </c>
-      <c r="F107" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>140</v>
-      </c>
-      <c r="B108" t="s">
-        <v>2</v>
-      </c>
-      <c r="C108" t="s">
-        <v>6</v>
-      </c>
-      <c r="D108" t="s">
-        <v>108</v>
-      </c>
-      <c r="E108" t="s">
-        <v>11</v>
-      </c>
-      <c r="F108" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>141</v>
-      </c>
-      <c r="B109" t="s">
-        <v>2</v>
-      </c>
-      <c r="C109" t="s">
-        <v>6</v>
-      </c>
-      <c r="D109" t="s">
-        <v>83</v>
-      </c>
-      <c r="E109" t="s">
-        <v>11</v>
-      </c>
-      <c r="F109" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>142</v>
-      </c>
-      <c r="B110" t="s">
-        <v>2</v>
-      </c>
-      <c r="C110" t="s">
-        <v>6</v>
-      </c>
-      <c r="D110" t="s">
-        <v>108</v>
-      </c>
-      <c r="E110" t="s">
-        <v>11</v>
-      </c>
-      <c r="F110" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>143</v>
-      </c>
-      <c r="B111" t="s">
-        <v>2</v>
-      </c>
-      <c r="C111" t="s">
-        <v>6</v>
-      </c>
-      <c r="D111" t="s">
-        <v>108</v>
-      </c>
-      <c r="E111" t="s">
-        <v>162</v>
-      </c>
-      <c r="F111" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>144</v>
       </c>
       <c r="B112" t="s">
         <v>2</v>
@@ -3177,15 +3190,15 @@
         <v>108</v>
       </c>
       <c r="E112" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F112" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B113" t="s">
         <v>2</v>
@@ -3194,18 +3207,18 @@
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E113" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="F113" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B114" t="s">
         <v>2</v>
@@ -3214,7 +3227,7 @@
         <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E114" t="s">
         <v>11</v>
@@ -3223,9 +3236,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="B115" t="s">
         <v>2</v>
@@ -3234,7 +3247,7 @@
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="E115" t="s">
         <v>11</v>
@@ -3243,9 +3256,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B116" t="s">
         <v>2</v>
@@ -3254,7 +3267,7 @@
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E116" t="s">
         <v>11</v>
@@ -3263,9 +3276,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B117" t="s">
         <v>2</v>
@@ -3274,18 +3287,18 @@
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E117" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
       <c r="F117" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B118" t="s">
         <v>2</v>
@@ -3294,18 +3307,18 @@
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="E118" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F118" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B119" t="s">
         <v>2</v>
@@ -3314,7 +3327,7 @@
         <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="E119" t="s">
         <v>11</v>
@@ -3323,9 +3336,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B120" t="s">
         <v>2</v>
@@ -3334,7 +3347,7 @@
         <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="E120" t="s">
         <v>11</v>
@@ -3343,9 +3356,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="B121" t="s">
         <v>2</v>
@@ -3354,7 +3367,7 @@
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="E121" t="s">
         <v>11</v>
@@ -3363,9 +3376,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B122" t="s">
         <v>2</v>
@@ -3374,7 +3387,7 @@
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="E122" t="s">
         <v>11</v>
@@ -3383,9 +3396,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B123" t="s">
         <v>2</v>
@@ -3394,7 +3407,7 @@
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>155</v>
+        <v>67</v>
       </c>
       <c r="E123" t="s">
         <v>11</v>
@@ -3403,9 +3416,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B124" t="s">
         <v>2</v>
@@ -3414,7 +3427,7 @@
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>155</v>
+        <v>14</v>
       </c>
       <c r="E124" t="s">
         <v>11</v>
@@ -3423,9 +3436,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B125" t="s">
         <v>2</v>
@@ -3434,7 +3447,7 @@
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>155</v>
+        <v>14</v>
       </c>
       <c r="E125" t="s">
         <v>11</v>
@@ -3443,9 +3456,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B126" t="s">
         <v>2</v>
@@ -3454,7 +3467,7 @@
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>155</v>
+        <v>40</v>
       </c>
       <c r="E126" t="s">
         <v>11</v>
@@ -3463,9 +3476,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B127" t="s">
         <v>2</v>
@@ -3474,7 +3487,7 @@
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>155</v>
+        <v>40</v>
       </c>
       <c r="E127" t="s">
         <v>11</v>
@@ -3483,9 +3496,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B128" t="s">
         <v>2</v>
@@ -3494,7 +3507,7 @@
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E128" t="s">
         <v>11</v>
@@ -3503,9 +3516,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B129" t="s">
         <v>2</v>
@@ -3514,7 +3527,7 @@
         <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="E129" t="s">
         <v>11</v>
@@ -3523,9 +3536,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B130" t="s">
         <v>2</v>
@@ -3534,18 +3547,18 @@
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>50</v>
+        <v>155</v>
       </c>
       <c r="E130" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F130" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B131" t="s">
         <v>2</v>
@@ -3554,7 +3567,7 @@
         <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="E131" t="s">
         <v>11</v>
@@ -3563,9 +3576,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B132" t="s">
         <v>2</v>
@@ -3574,18 +3587,18 @@
         <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="E132" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F132" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B133" t="s">
         <v>2</v>
@@ -3594,18 +3607,18 @@
         <v>6</v>
       </c>
       <c r="D133" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="E133" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F133" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B134" t="s">
         <v>2</v>
@@ -3614,12 +3627,132 @@
         <v>6</v>
       </c>
       <c r="D134" t="s">
+        <v>14</v>
+      </c>
+      <c r="E134" t="s">
+        <v>11</v>
+      </c>
+      <c r="F134" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>168</v>
+      </c>
+      <c r="B135" t="s">
+        <v>2</v>
+      </c>
+      <c r="C135" t="s">
+        <v>6</v>
+      </c>
+      <c r="D135" t="s">
+        <v>14</v>
+      </c>
+      <c r="E135" t="s">
+        <v>11</v>
+      </c>
+      <c r="F135" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>163</v>
+      </c>
+      <c r="B136" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136" t="s">
+        <v>6</v>
+      </c>
+      <c r="D136" t="s">
         <v>50</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E136" t="s">
+        <v>10</v>
+      </c>
+      <c r="F136" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>164</v>
+      </c>
+      <c r="B137" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137" t="s">
+        <v>6</v>
+      </c>
+      <c r="D137" t="s">
+        <v>108</v>
+      </c>
+      <c r="E137" t="s">
+        <v>11</v>
+      </c>
+      <c r="F137" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>165</v>
+      </c>
+      <c r="B138" t="s">
+        <v>2</v>
+      </c>
+      <c r="C138" t="s">
+        <v>6</v>
+      </c>
+      <c r="D138" t="s">
+        <v>86</v>
+      </c>
+      <c r="E138" t="s">
+        <v>10</v>
+      </c>
+      <c r="F138" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>166</v>
+      </c>
+      <c r="B139" t="s">
+        <v>2</v>
+      </c>
+      <c r="C139" t="s">
+        <v>6</v>
+      </c>
+      <c r="D139" t="s">
+        <v>14</v>
+      </c>
+      <c r="E139" t="s">
+        <v>10</v>
+      </c>
+      <c r="F139" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>169</v>
+      </c>
+      <c r="B140" t="s">
+        <v>2</v>
+      </c>
+      <c r="C140" t="s">
+        <v>6</v>
+      </c>
+      <c r="D140" t="s">
+        <v>50</v>
+      </c>
+      <c r="E140" t="s">
         <v>162</v>
       </c>
-      <c r="F134" t="s">
+      <c r="F140" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📝 added new parameters and variables
</commit_message>
<xml_diff>
--- a/01_EFForTS-ABM/EFForTS-ABM_parameters_and_output.xlsx
+++ b/01_EFForTS-ABM/EFForTS-ABM_parameters_and_output.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuliaHenzler\Documents\5_GitHub\EFForTS-ABM\01_EFForTS-ABM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1068FF-AFB2-41B5-9FD9-0F372F0456E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B934FD07-7CD4-4EE2-BA63-5C04C8EE12D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27150" yWindow="1430" windowWidth="18170" windowHeight="18060" xr2:uid="{CCAD1C1C-E277-4675-834D-1499CE7B176B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="183">
   <si>
     <t>group</t>
   </si>
@@ -555,9 +555,6 @@
     <t>biodiv_invest_objective</t>
   </si>
   <si>
-    <t>"generell"</t>
-  </si>
-  <si>
     <t>ecol_biodiv_interval</t>
   </si>
   <si>
@@ -570,16 +567,13 @@
     <t xml:space="preserve">patches </t>
   </si>
   <si>
-    <t>p_habitat_quality</t>
-  </si>
-  <si>
-    <t>landscape-hq</t>
-  </si>
-  <si>
-    <t>impact_all</t>
-  </si>
-  <si>
-    <t>dist_max</t>
+    <t>"general"</t>
+  </si>
+  <si>
+    <t>which-machine?</t>
+  </si>
+  <si>
+    <t>"server"</t>
   </si>
 </sst>
 </file>
@@ -940,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9AA953-A8CF-47CE-B234-B31FEC912566}">
-  <dimension ref="A1:F140"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109:XFD109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2018,7 +2012,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B54" t="s">
         <v>1</v>
@@ -2093,12 +2087,12 @@
         <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B58" t="s">
         <v>1</v>
@@ -2110,10 +2104,10 @@
         <v>84</v>
       </c>
       <c r="E58" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -2698,16 +2692,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>182</v>
+        <v>119</v>
       </c>
       <c r="B88" t="s">
         <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D88" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="E88" t="s">
         <v>11</v>
@@ -2718,16 +2712,16 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="B89" t="s">
         <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D89" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="E89" t="s">
         <v>11</v>
@@ -2738,7 +2732,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B90" t="s">
         <v>2</v>
@@ -2758,7 +2752,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B91" t="s">
         <v>2</v>
@@ -2778,7 +2772,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B92" t="s">
         <v>2</v>
@@ -2787,7 +2781,7 @@
         <v>5</v>
       </c>
       <c r="D92" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E92" t="s">
         <v>11</v>
@@ -2798,7 +2792,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B93" t="s">
         <v>2</v>
@@ -2818,7 +2812,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B94" t="s">
         <v>2</v>
@@ -2827,7 +2821,7 @@
         <v>5</v>
       </c>
       <c r="D94" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="E94" t="s">
         <v>11</v>
@@ -2838,7 +2832,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B95" t="s">
         <v>2</v>
@@ -2858,7 +2852,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B96" t="s">
         <v>2</v>
@@ -2867,7 +2861,7 @@
         <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="E96" t="s">
         <v>11</v>
@@ -2878,7 +2872,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B97" t="s">
         <v>2</v>
@@ -2887,10 +2881,10 @@
         <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E97" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="F97" t="s">
         <v>12</v>
@@ -2898,7 +2892,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B98" t="s">
         <v>2</v>
@@ -2907,7 +2901,7 @@
         <v>5</v>
       </c>
       <c r="D98" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E98" t="s">
         <v>11</v>
@@ -2918,7 +2912,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B99" t="s">
         <v>2</v>
@@ -2927,10 +2921,10 @@
         <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="E99" t="s">
-        <v>161</v>
+        <v>11</v>
       </c>
       <c r="F99" t="s">
         <v>12</v>
@@ -2938,7 +2932,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B100" t="s">
         <v>2</v>
@@ -2947,7 +2941,7 @@
         <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E100" t="s">
         <v>11</v>
@@ -2958,7 +2952,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B101" t="s">
         <v>2</v>
@@ -2978,7 +2972,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B102" t="s">
         <v>2</v>
@@ -2987,7 +2981,7 @@
         <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="E102" t="s">
         <v>11</v>
@@ -2998,7 +2992,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B103" t="s">
         <v>2</v>
@@ -3018,7 +3012,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B104" t="s">
         <v>2</v>
@@ -3038,7 +3032,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B105" t="s">
         <v>2</v>
@@ -3058,7 +3052,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B106" t="s">
         <v>2</v>
@@ -3078,7 +3072,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="B107" t="s">
         <v>2</v>
@@ -3087,7 +3081,7 @@
         <v>5</v>
       </c>
       <c r="D107" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="E107" t="s">
         <v>11</v>
@@ -3098,36 +3092,36 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="B108" t="s">
         <v>2</v>
       </c>
       <c r="C108" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
       <c r="D108" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="E108" t="s">
-        <v>11</v>
-      </c>
-      <c r="F108" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="F108" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="B109" t="s">
         <v>2</v>
       </c>
       <c r="C109" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D109" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="E109" t="s">
         <v>11</v>
@@ -3138,36 +3132,36 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="B110" t="s">
         <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>180</v>
+        <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="E110" t="s">
-        <v>17</v>
-      </c>
-      <c r="F110" t="b">
-        <v>0</v>
+        <v>161</v>
+      </c>
+      <c r="F110" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="B111" t="s">
         <v>2</v>
       </c>
       <c r="C111" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="E111" t="s">
         <v>11</v>
@@ -3178,7 +3172,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B112" t="s">
         <v>2</v>
@@ -3187,7 +3181,7 @@
         <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="E112" t="s">
         <v>11</v>
@@ -3198,7 +3192,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B113" t="s">
         <v>2</v>
@@ -3210,7 +3204,7 @@
         <v>108</v>
       </c>
       <c r="E113" t="s">
-        <v>161</v>
+        <v>11</v>
       </c>
       <c r="F113" t="s">
         <v>12</v>
@@ -3218,7 +3212,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B114" t="s">
         <v>2</v>
@@ -3230,7 +3224,7 @@
         <v>108</v>
       </c>
       <c r="E114" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
       <c r="F114" t="s">
         <v>12</v>
@@ -3238,7 +3232,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B115" t="s">
         <v>2</v>
@@ -3247,10 +3241,10 @@
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="E115" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F115" t="s">
         <v>12</v>
@@ -3258,7 +3252,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B116" t="s">
         <v>2</v>
@@ -3267,7 +3261,7 @@
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="E116" t="s">
         <v>11</v>
@@ -3278,7 +3272,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B117" t="s">
         <v>2</v>
@@ -3287,10 +3281,10 @@
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="E117" t="s">
-        <v>162</v>
+        <v>11</v>
       </c>
       <c r="F117" t="s">
         <v>12</v>
@@ -3298,7 +3292,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="B118" t="s">
         <v>2</v>
@@ -3307,10 +3301,10 @@
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="E118" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F118" t="s">
         <v>12</v>
@@ -3318,7 +3312,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B119" t="s">
         <v>2</v>
@@ -3338,7 +3332,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B120" t="s">
         <v>2</v>
@@ -3358,7 +3352,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B121" t="s">
         <v>2</v>
@@ -3367,7 +3361,7 @@
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="E121" t="s">
         <v>11</v>
@@ -3378,7 +3372,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B122" t="s">
         <v>2</v>
@@ -3387,7 +3381,7 @@
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="E122" t="s">
         <v>11</v>
@@ -3398,7 +3392,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B123" t="s">
         <v>2</v>
@@ -3407,7 +3401,7 @@
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="E123" t="s">
         <v>11</v>
@@ -3418,7 +3412,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B124" t="s">
         <v>2</v>
@@ -3427,7 +3421,7 @@
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E124" t="s">
         <v>11</v>
@@ -3438,7 +3432,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B125" t="s">
         <v>2</v>
@@ -3447,7 +3441,7 @@
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E125" t="s">
         <v>11</v>
@@ -3458,7 +3452,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B126" t="s">
         <v>2</v>
@@ -3467,7 +3461,7 @@
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="E126" t="s">
         <v>11</v>
@@ -3478,7 +3472,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B127" t="s">
         <v>2</v>
@@ -3487,7 +3481,7 @@
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="E127" t="s">
         <v>11</v>
@@ -3498,7 +3492,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B128" t="s">
         <v>2</v>
@@ -3507,7 +3501,7 @@
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="E128" t="s">
         <v>11</v>
@@ -3518,7 +3512,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B129" t="s">
         <v>2</v>
@@ -3538,7 +3532,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B130" t="s">
         <v>2</v>
@@ -3558,7 +3552,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B131" t="s">
         <v>2</v>
@@ -3567,7 +3561,7 @@
         <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>155</v>
+        <v>14</v>
       </c>
       <c r="E131" t="s">
         <v>11</v>
@@ -3578,7 +3572,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="B132" t="s">
         <v>2</v>
@@ -3587,7 +3581,7 @@
         <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>155</v>
+        <v>14</v>
       </c>
       <c r="E132" t="s">
         <v>11</v>
@@ -3598,7 +3592,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B133" t="s">
         <v>2</v>
@@ -3607,10 +3601,10 @@
         <v>6</v>
       </c>
       <c r="D133" t="s">
-        <v>155</v>
+        <v>50</v>
       </c>
       <c r="E133" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F133" t="s">
         <v>12</v>
@@ -3618,7 +3612,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B134" t="s">
         <v>2</v>
@@ -3627,7 +3621,7 @@
         <v>6</v>
       </c>
       <c r="D134" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="E134" t="s">
         <v>11</v>
@@ -3638,7 +3632,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B135" t="s">
         <v>2</v>
@@ -3647,10 +3641,10 @@
         <v>6</v>
       </c>
       <c r="D135" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="E135" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F135" t="s">
         <v>12</v>
@@ -3658,7 +3652,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B136" t="s">
         <v>2</v>
@@ -3667,7 +3661,7 @@
         <v>6</v>
       </c>
       <c r="D136" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="E136" t="s">
         <v>10</v>
@@ -3678,7 +3672,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B137" t="s">
         <v>2</v>
@@ -3687,72 +3681,12 @@
         <v>6</v>
       </c>
       <c r="D137" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="E137" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
       <c r="F137" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
-        <v>165</v>
-      </c>
-      <c r="B138" t="s">
-        <v>2</v>
-      </c>
-      <c r="C138" t="s">
-        <v>6</v>
-      </c>
-      <c r="D138" t="s">
-        <v>86</v>
-      </c>
-      <c r="E138" t="s">
-        <v>10</v>
-      </c>
-      <c r="F138" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
-        <v>166</v>
-      </c>
-      <c r="B139" t="s">
-        <v>2</v>
-      </c>
-      <c r="C139" t="s">
-        <v>6</v>
-      </c>
-      <c r="D139" t="s">
-        <v>14</v>
-      </c>
-      <c r="E139" t="s">
-        <v>10</v>
-      </c>
-      <c r="F139" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
-        <v>169</v>
-      </c>
-      <c r="B140" t="s">
-        <v>2</v>
-      </c>
-      <c r="C140" t="s">
-        <v>6</v>
-      </c>
-      <c r="D140" t="s">
-        <v>50</v>
-      </c>
-      <c r="E140" t="s">
-        <v>162</v>
-      </c>
-      <c r="F140" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>